<commit_message>
Update matching pipeline and add cleaner for each data file
</commit_message>
<xml_diff>
--- a/app/db/mapping/export/export_mapping_template.xlsx
+++ b/app/db/mapping/export/export_mapping_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidding/Desktop/East_Asia_Econ/econ_db/app/db/mapping/export/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidding/Desktop/East_Asia_Econ/econ-db/app/db/mapping/export/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{323AF2D2-668B-0C4D-B41A-79EC7E56132F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC0335FC-02CC-A743-85CC-3F1D9506E048}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{A991E29A-45E2-0240-B694-FA6F5C4458BA}"/>
+    <workbookView xWindow="-38400" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{A991E29A-45E2-0240-B694-FA6F5C4458BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="51">
   <si>
     <t>Main_category</t>
   </si>
@@ -176,19 +175,37 @@
   </si>
   <si>
     <t>Index, % MoM, SA</t>
+  </si>
+  <si>
+    <t>% of total</t>
+  </si>
+  <si>
+    <t>% of total, SA</t>
+  </si>
+  <si>
+    <t>% of GDP</t>
+  </si>
+  <si>
+    <t>% of GDP, SA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFCDD2E9"/>
+      <name val="Courier New"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -211,7 +228,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -219,6 +236,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -533,10 +551,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13CE9EA6-CAED-C544-94E6-9946C44D1FC0}">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -751,20 +769,43 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D17" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D18" t="s">
         <v>45</v>
       </c>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D19" t="s">
         <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="D20" t="s">
+        <v>47</v>
+      </c>
+      <c r="L20" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="D21" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="D22" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="23" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="D23" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add JP export m cleaner and matching mapping and renew gdp mapping template
</commit_message>
<xml_diff>
--- a/app/db/mapping/export/export_mapping_template.xlsx
+++ b/app/db/mapping/export/export_mapping_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidding/Desktop/East_Asia_Econ/econ-db/app/db/mapping/export/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC0335FC-02CC-A743-85CC-3F1D9506E048}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0810140E-8115-3041-B091-62C8A8F21586}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{A991E29A-45E2-0240-B694-FA6F5C4458BA}"/>
   </bookViews>
@@ -105,36 +105,24 @@
     <t>LCU</t>
   </si>
   <si>
-    <t>Index</t>
-  </si>
-  <si>
     <t>USD, % YoY</t>
   </si>
   <si>
     <t>LCU, % YoY</t>
   </si>
   <si>
-    <t>Index, % YoY</t>
-  </si>
-  <si>
     <t>USD, SA</t>
   </si>
   <si>
     <t>LCU, SA</t>
   </si>
   <si>
-    <t>Index, SA</t>
-  </si>
-  <si>
     <t>USD, % MoM</t>
   </si>
   <si>
     <t>LCU, % MoM</t>
   </si>
   <si>
-    <t>Index, % MoM</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
@@ -165,18 +153,12 @@
     <t>LCU, % YoY, SA</t>
   </si>
   <si>
-    <t>Index, % YoY, SA</t>
-  </si>
-  <si>
     <t>USD, % MoM, SA</t>
   </si>
   <si>
     <t>LCU, % MoM, SA</t>
   </si>
   <si>
-    <t>Index, % MoM, SA</t>
-  </si>
-  <si>
     <t>% of total</t>
   </si>
   <si>
@@ -187,6 +169,24 @@
   </si>
   <si>
     <t>% of GDP, SA</t>
+  </si>
+  <si>
+    <t>index</t>
+  </si>
+  <si>
+    <t>index, % YoY</t>
+  </si>
+  <si>
+    <t>index, SA</t>
+  </si>
+  <si>
+    <t>index, % MoM</t>
+  </si>
+  <si>
+    <t>index, % YoY, SA</t>
+  </si>
+  <si>
+    <t>index, % MoM, SA</t>
   </si>
 </sst>
 </file>
@@ -554,7 +554,7 @@
   <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -568,10 +568,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -591,13 +591,13 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D2" t="s">
         <v>21</v>
       </c>
       <c r="E2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F2">
         <v>4</v>
@@ -611,7 +611,7 @@
         <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D3" t="s">
         <v>22</v>
@@ -628,13 +628,13 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" t="s">
         <v>35</v>
       </c>
-      <c r="C4" t="s">
-        <v>39</v>
-      </c>
       <c r="D4" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>9</v>
@@ -645,7 +645,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>10</v>
@@ -656,7 +656,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>20</v>
@@ -667,10 +667,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D7" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="F7">
         <v>5</v>
@@ -678,7 +678,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>11</v>
@@ -689,7 +689,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>12</v>
@@ -700,7 +700,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D10" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>14</v>
@@ -711,7 +711,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D11" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>15</v>
@@ -722,7 +722,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D12" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>16</v>
@@ -733,7 +733,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D13" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>17</v>
@@ -744,7 +744,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D14" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>18</v>
@@ -755,7 +755,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D15" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>19</v>
@@ -766,46 +766,46 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D16" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D17" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D18" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E18" s="1"/>
     </row>
     <row r="19" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D19" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D20" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D21" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D22" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D23" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update export mapping template and matching results
</commit_message>
<xml_diff>
--- a/app/db/mapping/export/export_mapping_template.xlsx
+++ b/app/db/mapping/export/export_mapping_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidding/Desktop/East_Asia_Econ/econ-db/app/db/mapping/export/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0810140E-8115-3041-B091-62C8A8F21586}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34F94EF6-E0FA-CE47-B76D-FD6AB7FC6508}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{A991E29A-45E2-0240-B694-FA6F5C4458BA}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>Main_category</t>
   </si>
@@ -554,7 +554,7 @@
   <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -789,9 +789,7 @@
       <c r="D20" t="s">
         <v>41</v>
       </c>
-      <c r="L20" s="3" t="s">
-        <v>43</v>
-      </c>
+      <c r="L20" s="3"/>
     </row>
     <row r="21" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D21" t="s">

</xml_diff>

<commit_message>
Add onboarding process instruction
</commit_message>
<xml_diff>
--- a/app/db/mapping/export/export_mapping_template.xlsx
+++ b/app/db/mapping/export/export_mapping_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidding/Desktop/East_Asia_Econ/econ-db/app/db/mapping/export/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34F94EF6-E0FA-CE47-B76D-FD6AB7FC6508}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C33203C6-A97B-EA48-89A5-AF83E4DCBFF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{A991E29A-45E2-0240-B694-FA6F5C4458BA}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="30240" windowHeight="19640" xr2:uid="{A991E29A-45E2-0240-B694-FA6F5C4458BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -554,7 +554,7 @@
   <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Revert "Merge pull request #29 from Paul-Edward-C/add-cleaning-pipeline"
This reverts commit 6103128b1c95f93c8f062ada9f4d75b6fab77abb, reversing
changes made to 399dfe204bff0db336038295d726b3fdce98a9fc.
</commit_message>
<xml_diff>
--- a/app/db/mapping/export/export_mapping_template.xlsx
+++ b/app/db/mapping/export/export_mapping_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidding/Desktop/East_Asia_Econ/econ-db/app/db/mapping/export/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C33203C6-A97B-EA48-89A5-AF83E4DCBFF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34F94EF6-E0FA-CE47-B76D-FD6AB7FC6508}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="30240" windowHeight="19640" xr2:uid="{A991E29A-45E2-0240-B694-FA6F5C4458BA}"/>
+    <workbookView xWindow="-38400" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{A991E29A-45E2-0240-B694-FA6F5C4458BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -554,7 +554,7 @@
   <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Revert "Revert "Merge pull request #29 from Paul-Edward-C/add-cleaning-pipeline""
This reverts commit 92dbbddd0b1122e07625a0b97f822f4a67920fb0.
</commit_message>
<xml_diff>
--- a/app/db/mapping/export/export_mapping_template.xlsx
+++ b/app/db/mapping/export/export_mapping_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidding/Desktop/East_Asia_Econ/econ-db/app/db/mapping/export/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34F94EF6-E0FA-CE47-B76D-FD6AB7FC6508}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C33203C6-A97B-EA48-89A5-AF83E4DCBFF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{A991E29A-45E2-0240-B694-FA6F5C4458BA}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="30240" windowHeight="19640" xr2:uid="{A991E29A-45E2-0240-B694-FA6F5C4458BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -554,7 +554,7 @@
   <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>